<commit_message>
label based delay support + tests
</commit_message>
<xml_diff>
--- a/chapas_schedule_cemi.xlsx
+++ b/chapas_schedule_cemi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpern\Documents\GitHub\PyFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D8CBB6-8EAE-4DE3-BD6C-4AB0FBAFD66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76982DD-2308-44BC-9C48-45C0155E5D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,7 +677,7 @@
   <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F99" sqref="F2:F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>